<commit_message>
Tamanho do formulário ajeitado
</commit_message>
<xml_diff>
--- a/WindowsApplication1/Significado dos índices.xlsx
+++ b/WindowsApplication1/Significado dos índices.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="16608" windowHeight="9432"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="16608" windowHeight="9432" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="66">
   <si>
     <t xml:space="preserve">Label </t>
   </si>
@@ -166,6 +166,57 @@
   </si>
   <si>
     <t>comboBox16</t>
+  </si>
+  <si>
+    <t>Formulário</t>
+  </si>
+  <si>
+    <t>Tipo de Barra</t>
+  </si>
+  <si>
+    <t>Atributo</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>IDcasoBase</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Transmissão</t>
+  </si>
+  <si>
+    <t>Distribuição</t>
+  </si>
+  <si>
+    <t>SIM</t>
+  </si>
+  <si>
+    <t>Inserir</t>
+  </si>
+  <si>
+    <t>Remover</t>
+  </si>
+  <si>
+    <t>Atualizar</t>
+  </si>
+  <si>
+    <t>Pesquisar</t>
+  </si>
+  <si>
+    <t>TextBox</t>
+  </si>
+  <si>
+    <t>ComboBox</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Textbox</t>
   </si>
 </sst>
 </file>
@@ -188,7 +239,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,8 +270,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -243,11 +300,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -266,6 +360,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1167,12 +1285,127 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="24" style="9" customWidth="1"/>
+    <col min="2" max="2" width="16" style="9" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" style="9" customWidth="1"/>
+    <col min="5" max="8" width="17.33203125" style="9" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="13"/>
+      <c r="B3" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="15"/>
+      <c r="B4" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A4"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>

<commit_message>
case insert trans feito
</commit_message>
<xml_diff>
--- a/WindowsApplication1/Significado dos índices.xlsx
+++ b/WindowsApplication1/Significado dos índices.xlsx
@@ -513,7 +513,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -575,7 +575,7 @@
         <v>19</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="1">
         <v>5</v>
@@ -595,7 +595,7 @@
         <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1">
         <v>5</v>

</xml_diff>

<commit_message>
metade do insert de bus
</commit_message>
<xml_diff>
--- a/WindowsApplication1/Significado dos índices.xlsx
+++ b/WindowsApplication1/Significado dos índices.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
   <si>
     <t xml:space="preserve">Label </t>
   </si>
@@ -97,6 +97,126 @@
   </si>
   <si>
     <t>trans/case/insert</t>
+  </si>
+  <si>
+    <t>label7</t>
+  </si>
+  <si>
+    <t>case</t>
+  </si>
+  <si>
+    <t>combobox3</t>
+  </si>
+  <si>
+    <t>trans/bus/insert</t>
+  </si>
+  <si>
+    <t>label8</t>
+  </si>
+  <si>
+    <t>Número da barra</t>
+  </si>
+  <si>
+    <t>textbox1</t>
+  </si>
+  <si>
+    <t>label9</t>
+  </si>
+  <si>
+    <t>Número sequencial</t>
+  </si>
+  <si>
+    <t>textbox8</t>
+  </si>
+  <si>
+    <t>label10</t>
+  </si>
+  <si>
+    <t>magnitude de tensão</t>
+  </si>
+  <si>
+    <t>textbox2</t>
+  </si>
+  <si>
+    <t>label11</t>
+  </si>
+  <si>
+    <t>ângulo de fase</t>
+  </si>
+  <si>
+    <t>textbox12</t>
+  </si>
+  <si>
+    <t>base de tensão</t>
+  </si>
+  <si>
+    <t>label12</t>
+  </si>
+  <si>
+    <t>textbox3</t>
+  </si>
+  <si>
+    <t>tensão especificada</t>
+  </si>
+  <si>
+    <t>label16</t>
+  </si>
+  <si>
+    <t>textbox11</t>
+  </si>
+  <si>
+    <t>lim max geração</t>
+  </si>
+  <si>
+    <t>label19</t>
+  </si>
+  <si>
+    <t>textbox4</t>
+  </si>
+  <si>
+    <t>label20</t>
+  </si>
+  <si>
+    <t>lim min. geração</t>
+  </si>
+  <si>
+    <t>label22</t>
+  </si>
+  <si>
+    <t>textbox9</t>
+  </si>
+  <si>
+    <t>label21</t>
+  </si>
+  <si>
+    <t>textbox7</t>
+  </si>
+  <si>
+    <t>lim max tensão</t>
+  </si>
+  <si>
+    <t>textbox10</t>
+  </si>
+  <si>
+    <t>lim min. tensão</t>
+  </si>
+  <si>
+    <t>label23</t>
+  </si>
+  <si>
+    <t>nome da barra</t>
+  </si>
+  <si>
+    <t>textbox13</t>
+  </si>
+  <si>
+    <t>label24</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>combobox4</t>
   </si>
 </sst>
 </file>
@@ -513,7 +633,7 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -688,134 +808,264 @@
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="2">
+        <v>6</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="2">
+        <v>6</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="2">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="2">
+        <v>6</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="A13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="2">
+        <v>6</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="A14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="2">
+        <v>6</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="2">
+        <v>6</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="2">
+        <v>6</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
+      <c r="A17" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="2">
+        <v>6</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
+      <c r="A18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="2">
+        <v>6</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="A19" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="2">
+        <v>6</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="A20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="2">
+        <v>6</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="A21" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="2">
+        <v>6</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" s="2"/>

</xml_diff>

<commit_message>
até a tabela 6 ok acho
</commit_message>
<xml_diff>
--- a/WindowsApplication1/Significado dos índices.xlsx
+++ b/WindowsApplication1/Significado dos índices.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="127">
   <si>
     <t xml:space="preserve">Label </t>
   </si>
@@ -271,6 +271,135 @@
   </si>
   <si>
     <t>trans/busbustyperel/insert</t>
+  </si>
+  <si>
+    <t>inicialBus</t>
+  </si>
+  <si>
+    <t>finalBus</t>
+  </si>
+  <si>
+    <t>sequencialNumber</t>
+  </si>
+  <si>
+    <t>resistence</t>
+  </si>
+  <si>
+    <t>reactance</t>
+  </si>
+  <si>
+    <t>susceptance</t>
+  </si>
+  <si>
+    <t>MVAratings#1</t>
+  </si>
+  <si>
+    <t>MVAratings#2</t>
+  </si>
+  <si>
+    <t>MVAratings#3</t>
+  </si>
+  <si>
+    <t>circuitNumber</t>
+  </si>
+  <si>
+    <t>label30</t>
+  </si>
+  <si>
+    <t>label31</t>
+  </si>
+  <si>
+    <t>label32</t>
+  </si>
+  <si>
+    <t>label33</t>
+  </si>
+  <si>
+    <t>label34</t>
+  </si>
+  <si>
+    <t>label39</t>
+  </si>
+  <si>
+    <t>label38</t>
+  </si>
+  <si>
+    <t>label37</t>
+  </si>
+  <si>
+    <t>label36</t>
+  </si>
+  <si>
+    <t>label35</t>
+  </si>
+  <si>
+    <t>label40</t>
+  </si>
+  <si>
+    <t>label42</t>
+  </si>
+  <si>
+    <t>label41</t>
+  </si>
+  <si>
+    <t>combobox9</t>
+  </si>
+  <si>
+    <t>combobox10</t>
+  </si>
+  <si>
+    <t>texbox15</t>
+  </si>
+  <si>
+    <t>texbox16</t>
+  </si>
+  <si>
+    <t>texbox17</t>
+  </si>
+  <si>
+    <t>texbox18</t>
+  </si>
+  <si>
+    <t>texbox19</t>
+  </si>
+  <si>
+    <t>texbox20</t>
+  </si>
+  <si>
+    <t>texbox21</t>
+  </si>
+  <si>
+    <t>texbox22</t>
+  </si>
+  <si>
+    <t>texbox23</t>
+  </si>
+  <si>
+    <t>trans/line/insert</t>
+  </si>
+  <si>
+    <t>button10</t>
+  </si>
+  <si>
+    <t>button11</t>
+  </si>
+  <si>
+    <t>clear</t>
+  </si>
+  <si>
+    <t>combobox11</t>
+  </si>
+  <si>
+    <t>combobox12</t>
+  </si>
+  <si>
+    <t>label43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FormNotUsed </t>
+  </si>
+  <si>
+    <t>trans/linespacing/insert</t>
   </si>
 </sst>
 </file>
@@ -684,10 +813,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1320,6 +1449,324 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" s="1">
+        <v>9</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D33" s="1">
+        <v>9</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" s="1">
+        <v>9</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" s="1">
+        <v>9</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D36" s="1">
+        <v>9</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D37" s="1">
+        <v>9</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" s="1">
+        <v>9</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D39" s="1">
+        <v>9</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D40" s="1">
+        <v>9</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D41" s="1">
+        <v>9</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="A42" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D42" s="1">
+        <v>9</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="A43" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D43" s="1">
+        <v>9</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D44" s="1">
+        <v>9</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" s="1">
+        <v>9</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" s="1">
+        <v>9</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2">
+        <v>10</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+      <c r="H47" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
mais duas tabelas, to fazendo a de perdas
</commit_message>
<xml_diff>
--- a/WindowsApplication1/Significado dos índices.xlsx
+++ b/WindowsApplication1/Significado dos índices.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="172">
   <si>
     <t xml:space="preserve">Label </t>
   </si>
@@ -436,6 +436,105 @@
   </si>
   <si>
     <t>richTextBox3</t>
+  </si>
+  <si>
+    <t>line</t>
+  </si>
+  <si>
+    <t>trans/linelineType/insert</t>
+  </si>
+  <si>
+    <t>label49</t>
+  </si>
+  <si>
+    <t>label50</t>
+  </si>
+  <si>
+    <t>label51</t>
+  </si>
+  <si>
+    <t>comboBox15</t>
+  </si>
+  <si>
+    <t>comboBox14</t>
+  </si>
+  <si>
+    <t>comboBox16</t>
+  </si>
+  <si>
+    <t>trans/lossozine/insert</t>
+  </si>
+  <si>
+    <t>lossZOne</t>
+  </si>
+  <si>
+    <t>submit</t>
+  </si>
+  <si>
+    <t>button14</t>
+  </si>
+  <si>
+    <t>button15</t>
+  </si>
+  <si>
+    <t>label52</t>
+  </si>
+  <si>
+    <t>label53</t>
+  </si>
+  <si>
+    <t>label54</t>
+  </si>
+  <si>
+    <t>label55</t>
+  </si>
+  <si>
+    <t>button16</t>
+  </si>
+  <si>
+    <t>comboBox17</t>
+  </si>
+  <si>
+    <t>textBox14</t>
+  </si>
+  <si>
+    <t>richTextBox4</t>
+  </si>
+  <si>
+    <t>textBox24</t>
+  </si>
+  <si>
+    <t>label57</t>
+  </si>
+  <si>
+    <t>label58</t>
+  </si>
+  <si>
+    <t>label59</t>
+  </si>
+  <si>
+    <t>button18</t>
+  </si>
+  <si>
+    <t>button19</t>
+  </si>
+  <si>
+    <t>busID</t>
+  </si>
+  <si>
+    <t>lossZoneID</t>
+  </si>
+  <si>
+    <t>comboBox18</t>
+  </si>
+  <si>
+    <t>comboBox19</t>
+  </si>
+  <si>
+    <t>comboBox20</t>
+  </si>
+  <si>
+    <t>trans/losszoneBus/insert</t>
   </si>
 </sst>
 </file>
@@ -849,10 +948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1762,6 +1861,278 @@
       </c>
       <c r="E53" s="2" t="s">
         <v>129</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D54" s="1">
+        <v>13</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D55" s="1">
+        <v>13</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D56" s="1">
+        <v>13</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D57" s="1">
+        <v>13</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D58" s="1">
+        <v>13</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D59" s="2">
+        <v>14</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D60" s="2">
+        <v>14</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D61" s="2">
+        <v>14</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D62" s="2">
+        <v>14</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D63" s="2">
+        <v>14</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D64" s="2">
+        <v>14</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D65" s="1">
+        <v>15</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D66" s="1">
+        <v>15</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D67" s="1">
+        <v>15</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D68" s="1">
+        <v>15</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D69" s="1">
+        <v>15</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modelo de carga feito insert
</commit_message>
<xml_diff>
--- a/WindowsApplication1/Significado dos índices.xlsx
+++ b/WindowsApplication1/Significado dos índices.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="185">
   <si>
     <t xml:space="preserve">Label </t>
   </si>
@@ -525,16 +525,55 @@
     <t>lossZoneID</t>
   </si>
   <si>
-    <t>comboBox18</t>
-  </si>
-  <si>
-    <t>comboBox19</t>
-  </si>
-  <si>
-    <t>comboBox20</t>
-  </si>
-  <si>
     <t>trans/losszoneBus/insert</t>
+  </si>
+  <si>
+    <t>comboBox18;</t>
+  </si>
+  <si>
+    <t>comboBox19;</t>
+  </si>
+  <si>
+    <t>comboBox20;</t>
+  </si>
+  <si>
+    <t>label62;</t>
+  </si>
+  <si>
+    <t>label61;</t>
+  </si>
+  <si>
+    <t>label60;</t>
+  </si>
+  <si>
+    <t>ramo</t>
+  </si>
+  <si>
+    <t>losszone</t>
+  </si>
+  <si>
+    <t>button21;</t>
+  </si>
+  <si>
+    <t>button20;</t>
+  </si>
+  <si>
+    <t>comboBox23;</t>
+  </si>
+  <si>
+    <t>comboBox22;</t>
+  </si>
+  <si>
+    <t>comboBox21;</t>
+  </si>
+  <si>
+    <t>trans/losszoneLine/insert</t>
+  </si>
+  <si>
+    <t>label63</t>
+  </si>
+  <si>
+    <t>trans/modelload/insert</t>
   </si>
 </sst>
 </file>
@@ -948,10 +987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2058,13 +2097,13 @@
         <v>67</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D65" s="1">
         <v>15</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -2075,13 +2114,13 @@
         <v>166</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D66" s="1">
         <v>15</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -2092,13 +2131,13 @@
         <v>167</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D67" s="1">
         <v>15</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -2115,7 +2154,7 @@
         <v>15</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -2132,7 +2171,109 @@
         <v>15</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D70" s="2">
+        <v>16</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D71" s="2">
+        <v>16</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D72" s="2">
+        <v>16</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D73" s="2">
+        <v>16</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D74" s="2">
+        <v>16</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D75" s="1">
+        <v>17</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
case distr insert ok
</commit_message>
<xml_diff>
--- a/WindowsApplication1/Significado dos índices.xlsx
+++ b/WindowsApplication1/Significado dos índices.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="343">
   <si>
     <t xml:space="preserve">Label </t>
   </si>
@@ -1024,6 +1024,30 @@
   </si>
   <si>
     <t>richTextBox6;</t>
+  </si>
+  <si>
+    <t>label112;</t>
+  </si>
+  <si>
+    <t>textBox44;</t>
+  </si>
+  <si>
+    <t>richTextBox7;</t>
+  </si>
+  <si>
+    <t>label113;</t>
+  </si>
+  <si>
+    <t>distr/case/insert</t>
+  </si>
+  <si>
+    <t>button42;</t>
+  </si>
+  <si>
+    <t>título</t>
+  </si>
+  <si>
+    <t>button43;</t>
   </si>
 </sst>
 </file>
@@ -1437,10 +1461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E139"/>
+  <dimension ref="A1:E143"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="D135" sqref="D135"/>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="C140" sqref="C140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3812,6 +3836,74 @@
       </c>
       <c r="E139" s="1" t="s">
         <v>333</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
+      <c r="A140" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="D140" s="2">
+        <v>30</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
+      <c r="A141" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="D141" s="2">
+        <v>30</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5">
+      <c r="A142" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D142" s="2">
+        <v>30</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
+      <c r="A143" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D143" s="2">
+        <v>30</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>